<commit_message>
Update to test xlsx
</commit_message>
<xml_diff>
--- a/AutoTest_gitclassroom_tests.xlsx
+++ b/AutoTest_gitclassroom_tests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmt/Library/CloudStorage/Dropbox/UCA/Data Structures/source/Stack_Project/Stack_Project_AutoTest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelle/Dropbox/UCA/Data Structures/source/Stack_Project/Stack_Project_AutoTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DF6B41-B983-FB41-9BAD-293351C38957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8EB564-0313-BA45-B23F-B2C2049E3883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28680" yWindow="-16520" windowWidth="28140" windowHeight="24780" xr2:uid="{29F2130F-3E6E-6C43-8BD2-2E7492F933ED}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{29F2130F-3E6E-6C43-8BD2-2E7492F933ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Classroom" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t>AutoTest Setup</t>
   </si>
@@ -57,22 +57,7 @@
     <t>Points</t>
   </si>
   <si>
-    <t>git clone https://github.com/TeacherTalley/LinkedList_AutoTest.git</t>
-  </si>
-  <si>
-    <t>Install test code, copy student source, build student and test code</t>
-  </si>
-  <si>
-    <t>cd LinkedList_AutoTest &amp;&amp; ./AutoTest_setup.sh</t>
-  </si>
-  <si>
     <t>Main Output</t>
-  </si>
-  <si>
-    <t>./LinkedList_AutoTest/AutoTest_OutputTest.sh</t>
-  </si>
-  <si>
-    <t>Run student main and compare output to test</t>
   </si>
   <si>
     <t>Coding Style</t>
@@ -616,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D968784-9ABC-434B-B612-3087309D1BAB}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -652,101 +637,92 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E7">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E8">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E9">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E10">
         <v>10</v>
@@ -754,40 +730,42 @@
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>63</v>
+        <v>38</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="D12" t="s">
+        <v>10</v>
       </c>
       <c r="E12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>63</v>
+        <v>39</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="D13" t="s">
+        <v>13</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2"/>
       <c r="D14" t="s">
@@ -799,11 +777,11 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B15" s="2"/>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -811,11 +789,11 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2"/>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -823,11 +801,11 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B17" s="2"/>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -835,11 +813,11 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B18" s="2"/>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -847,11 +825,11 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2"/>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -859,11 +837,11 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B20" s="2"/>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -871,11 +849,11 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2"/>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -883,11 +861,11 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B22" s="2"/>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -895,11 +873,11 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2"/>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -907,7 +885,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2"/>
       <c r="D24" t="s">
@@ -919,11 +897,11 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B25" s="2"/>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -931,11 +909,11 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B26" s="2"/>
       <c r="D26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -943,11 +921,11 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B27" s="2"/>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -955,11 +933,11 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2"/>
       <c r="D28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -967,11 +945,11 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B29" s="2"/>
       <c r="D29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -979,11 +957,11 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B30" s="2"/>
       <c r="D30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -991,46 +969,22 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B31" s="2"/>
       <c r="D31" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="D32" t="s">
-        <v>32</v>
+      <c r="A32" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="D33" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E34">
-        <f>SUM(E3:E33)</f>
+        <f>SUM(E3:E31)</f>
         <v>100</v>
       </c>
     </row>
@@ -1068,10 +1022,10 @@
     </row>
     <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -1079,10 +1033,10 @@
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -1090,10 +1044,10 @@
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1101,10 +1055,10 @@
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1112,10 +1066,10 @@
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C6">
         <v>15</v>
@@ -1123,10 +1077,10 @@
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -1134,10 +1088,10 @@
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -1145,10 +1099,10 @@
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C9">
         <v>15</v>
@@ -1156,10 +1110,10 @@
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -1167,10 +1121,10 @@
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1178,10 +1132,10 @@
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1189,10 +1143,10 @@
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1200,10 +1154,10 @@
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -1211,10 +1165,10 @@
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -1222,10 +1176,10 @@
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -1233,10 +1187,10 @@
     </row>
     <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1244,7 +1198,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C18">
         <f>SUM(C2:C17)</f>

</xml_diff>